<commit_message>
Fake IP Nhung chưa test thử Fake được hay không
</commit_message>
<xml_diff>
--- a/Excel/Data.xlsx
+++ b/Excel/Data.xlsx
@@ -12,12 +12,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
-    <sheet name="TINH BINH DINH" sheetId="152" r:id="rId1"/>
-    <sheet name="TINH PHU YEN" sheetId="139" r:id="rId2"/>
-    <sheet name="TINH TAY NINH" sheetId="135" r:id="rId3"/>
-    <sheet name="QUAN 2" sheetId="115" r:id="rId4"/>
-    <sheet name="TINH LAM DONG" sheetId="113" r:id="rId5"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId6"/>
+    <sheet name="TINH BINH DINH" sheetId="6" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -29,27 +25,78 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
-  <si>
-    <t>22/04/2021</t>
-  </si>
-  <si>
-    <t>CÔNG TY TNHH LAMVIEN DALAT</t>
-  </si>
-  <si>
-    <t>Thôn 1, Xã Lộc Ngãi, Huyện Bảo Lâm, Tỉnh Lâm Đồng</t>
-  </si>
-  <si>
-    <t>NGUYỄN VĂN VIÊN</t>
-  </si>
-  <si>
-    <t>CÔNG TY TNHH NĂNG LƯỢNG CAMELLIA</t>
-  </si>
-  <si>
-    <t>Thôn 4, Xã Ma Đa Guôi, Huyện Đạ Huoai, Tỉnh Lâm Đồng</t>
-  </si>
-  <si>
-    <t>Hoàng Lan Chi</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+  <si>
+    <t>4101598746 - Công Ty TNHH Chế Biến Lâm Sản Phúc Khang</t>
+  </si>
+  <si>
+    <t>CÔNG TY TNHH CHẾ BIẾN LÂM SẢN PHÚC KHANG</t>
+  </si>
+  <si>
+    <t>Thôn Hưng Mỹ 1, Xã Cát Hưng, Huyện Phù Cát, Tỉnh Bình Định</t>
+  </si>
+  <si>
+    <t>Đào Thảo</t>
+  </si>
+  <si>
+    <t>4101598739 - Công Ty Cổ Phần Daily Feed Việt Nam</t>
+  </si>
+  <si>
+    <t>CÔNG TY CỔ PHẦN DAILY FEED VIỆT NAM</t>
+  </si>
+  <si>
+    <t>Đội 17, thôn Tư Cung, Xã Phước Thắng, Huyện Tuy Phước, Tỉnh Bình Định</t>
+  </si>
+  <si>
+    <t>Phạm Đình Tỵ</t>
+  </si>
+  <si>
+    <t>4101598721 - Công Ty TNHH Tổng Hợp Thương Mại Dịch Vụ Hoàng Phi</t>
+  </si>
+  <si>
+    <t>CÔNG TY TNHH TỔNG HỢP THƯƠNG MẠI DỊCH VỤ HOÀNG PHI</t>
+  </si>
+  <si>
+    <t>Số 168 Nguyễn Trác, Phường Nhơn Bình, Thành phố Quy Nhơn, Tỉnh Bình Định</t>
+  </si>
+  <si>
+    <t>Phạm Lê Hoàng Phi</t>
+  </si>
+  <si>
+    <t>4101598707 - Công Ty TNHH Kinh Doanh Tổng Hợp Phú An</t>
+  </si>
+  <si>
+    <t>CÔNG TY TNHH KINH DOANH TỔNG HỢP PHÚ AN</t>
+  </si>
+  <si>
+    <t>02 Cần Vương, Phường Nguyễn Văn Cừ, Thành phố Quy Nhơn, Tỉnh Bình Định</t>
+  </si>
+  <si>
+    <t>Trần Xuân Chí</t>
+  </si>
+  <si>
+    <t>4101598658 - Công Ty TNHH Gạch Tuy Nen Nhật Đức</t>
+  </si>
+  <si>
+    <t>CÔNG TY TNHH GẠCH TUY NEN NHẬT ĐỨC</t>
+  </si>
+  <si>
+    <t>Xóm Nam, thôn Lai Nghi, Xã Bình Nghi, Huyện Tây Sơn, Tỉnh Bình Định</t>
+  </si>
+  <si>
+    <t>Nguyễn Thị Tình</t>
+  </si>
+  <si>
+    <t>4101598665 - Công Ty TNHH Dịch Vụ Thương Mại Vận Tải Trung Nam</t>
+  </si>
+  <si>
+    <t>CÔNG TY TNHH DỊCH VỤ THƯƠNG MẠI VẬN TẢI TRUNG NAM</t>
+  </si>
+  <si>
+    <t>Thôn Bình Trị, Xã Mỹ Quang, Huyện Phù Mỹ, Tỉnh Bình Định</t>
+  </si>
+  <si>
+    <t>Nguyễn Trọng Khiêm</t>
   </si>
 </sst>
 </file>
@@ -368,109 +415,138 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>44261</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1">
+        <v>982776409</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1">
+        <v>44261</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2">
+        <v>972537148</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1">
+        <v>44233</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3">
+        <v>937712887</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1">
+        <v>44233</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4">
+        <v>977318399</v>
+      </c>
+      <c r="F4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1">
+        <v>44233</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5">
+        <v>399780288</v>
+      </c>
+      <c r="F5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="1">
+        <v>44233</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6">
+        <v>965154585</v>
+      </c>
+      <c r="F6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="16.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>5801462252</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1">
-        <v>979269067</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>5801462277</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2">
-        <v>383809916</v>
-      </c>
-      <c r="F2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B24:B50"/>
   <sheetViews>

</xml_diff>